<commit_message>
Fixed bom for Digikey
</commit_message>
<xml_diff>
--- a/Kicad files/OpenHVPS-4/OpenHVPS-4 BOM .xlsx
+++ b/Kicad files/OpenHVPS-4/OpenHVPS-4 BOM .xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
   <si>
     <t xml:space="preserve">Designator</t>
   </si>
@@ -67,7 +67,7 @@
     <t xml:space="preserve">D1 D2 </t>
   </si>
   <si>
-    <t xml:space="preserve">BAS16J135</t>
+    <t xml:space="preserve">BAS16J,135</t>
   </si>
   <si>
     <t xml:space="preserve">D3 D4 D5 D6 D7 D8 D9 </t>
@@ -82,19 +82,7 @@
     <t xml:space="preserve">FB1 FB2 </t>
   </si>
   <si>
-    <t xml:space="preserve">BKP2125HS221-T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">~</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1 </t>
+    <t xml:space="preserve">‎MH2029-221Y‎</t>
   </si>
   <si>
     <t xml:space="preserve">L1 </t>
@@ -217,7 +205,7 @@
     <t xml:space="preserve">U1 </t>
   </si>
   <si>
-    <t xml:space="preserve">MAX6008AEUR-T</t>
+    <t xml:space="preserve">MAX6008AEUR+TCT-ND‎</t>
   </si>
   <si>
     <t xml:space="preserve">U2 </t>
@@ -245,7 +233,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -275,12 +263,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FF3C3C3C"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -324,7 +306,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -334,10 +316,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -422,15 +400,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.09765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.11328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="76.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="68.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="8.36"/>
@@ -440,7 +418,7 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -451,7 +429,7 @@
       <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="n">
+      <c r="B2" s="3" t="n">
         <v>885012207111</v>
       </c>
       <c r="C2" s="0" t="n">
@@ -573,7 +551,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>1</v>
@@ -581,10 +559,10 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>1</v>
@@ -592,10 +570,10 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>1</v>
@@ -603,10 +581,10 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>1</v>
@@ -614,10 +592,10 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>1</v>
@@ -625,21 +603,21 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>1</v>
@@ -647,10 +625,10 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>1</v>
@@ -658,21 +636,21 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>1</v>
@@ -680,10 +658,10 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>1</v>
@@ -691,10 +669,10 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>1</v>
@@ -702,10 +680,10 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>1</v>
@@ -713,10 +691,10 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>1</v>
@@ -724,10 +702,10 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>1</v>
@@ -735,32 +713,32 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>1</v>
@@ -768,32 +746,32 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>1</v>
@@ -801,64 +779,34 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="C36" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="C37" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="C38" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0"/>
-      <c r="B39" s="0"/>
-      <c r="C39" s="0"/>
-    </row>
+      <c r="A36" s="0"/>
+      <c r="B36" s="0"/>
+      <c r="C36" s="0"/>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>